<commit_message>
new functions & bug fixes
</commit_message>
<xml_diff>
--- a/data/EngRus.xlsx
+++ b/data/EngRus.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">affect</t>
   </si>
   <si>
-    <t xml:space="preserve">влять, воздействовать</t>
+    <t xml:space="preserve">влиять, воздействовать</t>
   </si>
   <si>
     <t xml:space="preserve">agile</t>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">amount</t>
   </si>
   <si>
-    <t xml:space="preserve">количество, сумма составлять</t>
+    <t xml:space="preserve">количество, сумма, составлять</t>
   </si>
   <si>
     <t xml:space="preserve">ancestor</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">approach</t>
   </si>
   <si>
-    <t xml:space="preserve">подход(ить), приближение(ться)</t>
+    <t xml:space="preserve">подходить, приближение</t>
   </si>
   <si>
     <t xml:space="preserve">appropriate</t>
@@ -1392,9 +1392,9 @@
   <dimension ref="A1:B191"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A154" activeCellId="0" sqref="A154"/>
+      <selection pane="bottomLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
add support enter one word + gems
</commit_message>
<xml_diff>
--- a/data/EngRus.xlsx
+++ b/data/EngRus.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$223</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="446">
   <si>
     <t xml:space="preserve">ENG</t>
   </si>
@@ -28,6 +31,12 @@
     <t xml:space="preserve">RUS</t>
   </si>
   <si>
+    <t xml:space="preserve">about</t>
+  </si>
+  <si>
+    <t xml:space="preserve">примерно</t>
+  </si>
+  <si>
     <t xml:space="preserve">access</t>
   </si>
   <si>
@@ -46,6 +55,12 @@
     <t xml:space="preserve">Корректировка</t>
   </si>
   <si>
+    <t xml:space="preserve">adore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">обожать</t>
+  </si>
+  <si>
     <t xml:space="preserve">affect</t>
   </si>
   <si>
@@ -88,6 +103,12 @@
     <t xml:space="preserve">предок</t>
   </si>
   <si>
+    <t xml:space="preserve">anyone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">кого угодно</t>
+  </si>
+  <si>
     <t xml:space="preserve">appear</t>
   </si>
   <si>
@@ -112,6 +133,12 @@
     <t xml:space="preserve">произвольный, случайный</t>
   </si>
   <si>
+    <t xml:space="preserve">Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Район</t>
+  </si>
+  <si>
     <t xml:space="preserve">arise</t>
   </si>
   <si>
@@ -136,6 +163,12 @@
     <t xml:space="preserve">прикреплять, присоединять, стыковывать</t>
   </si>
   <si>
+    <t xml:space="preserve">best regards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">с уважением</t>
+  </si>
+  <si>
     <t xml:space="preserve">built-in</t>
   </si>
   <si>
@@ -166,6 +199,12 @@
     <t xml:space="preserve">комната, камера</t>
   </si>
   <si>
+    <t xml:space="preserve">Cheers!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ура!</t>
+  </si>
+  <si>
     <t xml:space="preserve">clause</t>
   </si>
   <si>
@@ -178,10 +217,16 @@
     <t xml:space="preserve">закрытие, завершение</t>
   </si>
   <si>
+    <t xml:space="preserve">coinsidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">стечение обстоятельств</t>
+  </si>
+  <si>
     <t xml:space="preserve">compare</t>
   </si>
   <si>
-    <t xml:space="preserve">сравни(ва)ть, сравнение</t>
+    <t xml:space="preserve">сравнивать, сравнение</t>
   </si>
   <si>
     <t xml:space="preserve">comparison</t>
@@ -262,6 +307,12 @@
     <t xml:space="preserve">мужество, смелость</t>
   </si>
   <si>
+    <t xml:space="preserve">crowd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">толпа</t>
+  </si>
+  <si>
     <t xml:space="preserve">decimate</t>
   </si>
   <si>
@@ -331,7 +382,7 @@
     <t xml:space="preserve">described</t>
   </si>
   <si>
-    <t xml:space="preserve">описано(ывать), охарактеризовывать</t>
+    <t xml:space="preserve">описывать, охарактеризовать</t>
   </si>
   <si>
     <t xml:space="preserve">deserve</t>
@@ -376,6 +427,12 @@
     <t xml:space="preserve">область, сфера</t>
   </si>
   <si>
+    <t xml:space="preserve">dough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тесто</t>
+  </si>
+  <si>
     <t xml:space="preserve">dye</t>
   </si>
   <si>
@@ -406,16 +463,22 @@
     <t xml:space="preserve">поощрять, ободрять, поддерживать</t>
   </si>
   <si>
+    <t xml:space="preserve">examinе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">исследовать, проверять</t>
+  </si>
+  <si>
     <t xml:space="preserve">examining</t>
   </si>
   <si>
     <t xml:space="preserve">исследующий</t>
   </si>
   <si>
-    <t xml:space="preserve">examinе</t>
-  </si>
-  <si>
-    <t xml:space="preserve">исследовать, проверять</t>
+    <t xml:space="preserve">exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">исключать</t>
   </si>
   <si>
     <t xml:space="preserve">executing</t>
@@ -439,13 +502,7 @@
     <t xml:space="preserve">explicitly</t>
   </si>
   <si>
-    <t xml:space="preserve">ясно, недвусмысленно</t>
-  </si>
-  <si>
-    <t xml:space="preserve">explicity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">явно</t>
+    <t xml:space="preserve">ясно, недвусмысленно, явно</t>
   </si>
   <si>
     <t xml:space="preserve">expression</t>
@@ -502,6 +559,12 @@
     <t xml:space="preserve">в дальнейшем, затем, более того</t>
   </si>
   <si>
+    <t xml:space="preserve">Going through</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Прохожу</t>
+  </si>
+  <si>
     <t xml:space="preserve">grasp</t>
   </si>
   <si>
@@ -511,7 +574,7 @@
     <t xml:space="preserve">guess</t>
   </si>
   <si>
-    <t xml:space="preserve">угадывать</t>
+    <t xml:space="preserve">угадывать, угадай</t>
   </si>
   <si>
     <t xml:space="preserve">handling</t>
@@ -550,6 +613,12 @@
     <t xml:space="preserve">неизгладимое впечатление</t>
   </si>
   <si>
+    <t xml:space="preserve">impudent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">наглый</t>
+  </si>
+  <si>
     <t xml:space="preserve">in addition</t>
   </si>
   <si>
@@ -568,6 +637,9 @@
     <t xml:space="preserve">неизгладимый</t>
   </si>
   <si>
+    <t xml:space="preserve">indelible impression</t>
+  </si>
+  <si>
     <t xml:space="preserve">indices</t>
   </si>
   <si>
@@ -610,13 +682,16 @@
     <t xml:space="preserve">осмотр, контроль</t>
   </si>
   <si>
+    <t xml:space="preserve">Inspiration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вдохновение</t>
+  </si>
+  <si>
     <t xml:space="preserve">instance</t>
   </si>
   <si>
-    <t xml:space="preserve">пример, образец</t>
-  </si>
-  <si>
-    <t xml:space="preserve">например</t>
+    <t xml:space="preserve">экземпляр, пример, образец, например</t>
   </si>
   <si>
     <t xml:space="preserve">instantiating</t>
@@ -679,13 +754,31 @@
     <t xml:space="preserve">вопрос, исход, результат, выдавать выпускать</t>
   </si>
   <si>
+    <t xml:space="preserve">it happens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">бывает</t>
+  </si>
+  <si>
+    <t xml:space="preserve">known</t>
+  </si>
+  <si>
+    <t xml:space="preserve">известен</t>
+  </si>
+  <si>
     <t xml:space="preserve">lack</t>
   </si>
   <si>
     <t xml:space="preserve">отсутствие</t>
   </si>
   <si>
-    <t xml:space="preserve">measure(ment)</t>
+    <t xml:space="preserve">light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">лёгкий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measurement</t>
   </si>
   <si>
     <t xml:space="preserve">измерять, мера, оценивать</t>
@@ -703,12 +796,36 @@
     <t xml:space="preserve">военная</t>
   </si>
   <si>
+    <t xml:space="preserve">military department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">военная кафедра</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more</t>
+  </si>
+  <si>
+    <t xml:space="preserve">подробнее</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multifarious tangled world</t>
+  </si>
+  <si>
+    <t xml:space="preserve">многообразный запутанный мир</t>
+  </si>
+  <si>
     <t xml:space="preserve">neither</t>
   </si>
   <si>
     <t xml:space="preserve">ни, ни один, никто</t>
   </si>
   <si>
+    <t xml:space="preserve">Nothing wrong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ничего страшного</t>
+  </si>
+  <si>
     <t xml:space="preserve">nurture</t>
   </si>
   <si>
@@ -727,10 +844,10 @@
     <t xml:space="preserve">одержимый</t>
   </si>
   <si>
-    <t xml:space="preserve">obtain(ed)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">получать(нный)</t>
+    <t xml:space="preserve">obtain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">получать</t>
   </si>
   <si>
     <t xml:space="preserve">odd</t>
@@ -760,10 +877,7 @@
     <t xml:space="preserve">order</t>
   </si>
   <si>
-    <t xml:space="preserve">порядок, последовательность, упорядоченность</t>
-  </si>
-  <si>
-    <t xml:space="preserve">заказ</t>
+    <t xml:space="preserve">заказ, порядок, последовательность, упорядоченность</t>
   </si>
   <si>
     <t xml:space="preserve">ordering</t>
@@ -790,6 +904,12 @@
     <t xml:space="preserve">в частности, особенно, в особенности, особым образом</t>
   </si>
   <si>
+    <t xml:space="preserve">Passed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Миновал</t>
+  </si>
+  <si>
     <t xml:space="preserve">permission</t>
   </si>
   <si>
@@ -820,10 +940,10 @@
     <t xml:space="preserve">проекция, наметка</t>
   </si>
   <si>
-    <t xml:space="preserve">proper(ly)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">правильный(но)</t>
+    <t xml:space="preserve">proper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">правильный</t>
   </si>
   <si>
     <t xml:space="preserve">propogation</t>
@@ -880,10 +1000,16 @@
     <t xml:space="preserve">получено, принятый</t>
   </si>
   <si>
-    <t xml:space="preserve">recieve(r)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">принимать, получать (+сущ.)</t>
+    <t xml:space="preserve">recieve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">принимать, получать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recipe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">рецепт</t>
   </si>
   <si>
     <t xml:space="preserve">recognize</t>
@@ -895,7 +1021,7 @@
     <t xml:space="preserve">rectifier</t>
   </si>
   <si>
-    <t xml:space="preserve">исправлять, выпрямлять, выпрямитель, декектор</t>
+    <t xml:space="preserve">исправлять, выпрямлять, выпрямитель, детектор</t>
   </si>
   <si>
     <t xml:space="preserve">reduce</t>
@@ -904,10 +1030,10 @@
     <t xml:space="preserve">уменьшить, снижать</t>
   </si>
   <si>
-    <t xml:space="preserve">refer(ring)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">относиться, обращатья(ссылаясь)</t>
+    <t xml:space="preserve">refer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">относиться, обращаться</t>
   </si>
   <si>
     <t xml:space="preserve">reference</t>
@@ -958,10 +1084,10 @@
     <t xml:space="preserve">строгий</t>
   </si>
   <si>
-    <t xml:space="preserve">sample(d)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">образец, пример, выборка(пробовать)</t>
+    <t xml:space="preserve">sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">образец, пример, выборка, случайный</t>
   </si>
   <si>
     <t xml:space="preserve">satisfy</t>
@@ -1045,18 +1171,48 @@
     <t xml:space="preserve">захват подстроки</t>
   </si>
   <si>
+    <t xml:space="preserve">suppose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">предполагать</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">уверен</t>
+  </si>
+  <si>
     <t xml:space="preserve">therefore</t>
   </si>
   <si>
     <t xml:space="preserve">поэтому, потому</t>
   </si>
   <si>
+    <t xml:space="preserve">This happens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Это бывает</t>
+  </si>
+  <si>
     <t xml:space="preserve">thus</t>
   </si>
   <si>
     <t xml:space="preserve">таким образом, поэтому</t>
   </si>
   <si>
+    <t xml:space="preserve">Tied up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Связана</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">жёсткий</t>
+  </si>
+  <si>
     <t xml:space="preserve">tracing</t>
   </si>
   <si>
@@ -1075,6 +1231,12 @@
     <t xml:space="preserve">очередь</t>
   </si>
   <si>
+    <t xml:space="preserve">turned up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">оказался</t>
+  </si>
+  <si>
     <t xml:space="preserve">undersample</t>
   </si>
   <si>
@@ -1093,12 +1255,24 @@
     <t xml:space="preserve">развязать</t>
   </si>
   <si>
+    <t xml:space="preserve">Until next letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">До следующего письма</t>
+  </si>
+  <si>
     <t xml:space="preserve">unwieldy</t>
   </si>
   <si>
     <t xml:space="preserve">громоздкий</t>
   </si>
   <si>
+    <t xml:space="preserve">vacation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">отпуск</t>
+  </si>
+  <si>
     <t xml:space="preserve">variation</t>
   </si>
   <si>
@@ -1129,6 +1303,24 @@
     <t xml:space="preserve">порочный</t>
   </si>
   <si>
+    <t xml:space="preserve">wallow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">барахтаться</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was engaged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Занимался</t>
+  </si>
+  <si>
+    <t xml:space="preserve">whatever</t>
+  </si>
+  <si>
+    <t xml:space="preserve">без разницы</t>
+  </si>
+  <si>
     <t xml:space="preserve">wherever</t>
   </si>
   <si>
@@ -1139,6 +1331,12 @@
   </si>
   <si>
     <t xml:space="preserve">будь то</t>
+  </si>
+  <si>
+    <t xml:space="preserve">which is</t>
+  </si>
+  <si>
+    <t xml:space="preserve">которая</t>
   </si>
   <si>
     <t xml:space="preserve">whoever</t>
@@ -1169,6 +1367,18 @@
       </rPr>
       <t xml:space="preserve">, весь</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You roll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Валяешься</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cause</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Причина, дело, повод, процесс</t>
   </si>
 </sst>
 </file>
@@ -1282,7 +1492,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1293,6 +1503,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1383,29 +1597,33 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <tabColor rgb="FF6D9EEB"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B191"/>
+  <dimension ref="A1:C225"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="B218" activeCellId="0" sqref="B218"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1446,7 +1664,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1465,7 +1683,7 @@
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1510,10 +1728,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1550,10 +1768,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1590,10 +1808,10 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="3" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1638,7 +1856,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B30" s="0" t="s">
@@ -1662,10 +1880,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1694,10 +1912,10 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="0" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1710,10 +1928,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="0" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1750,26 +1968,26 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="4" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="0" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1782,10 +2000,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="3" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1809,7 +2027,7 @@
       <c r="A51" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="0" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1822,10 +2040,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="4" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1873,23 +2091,23 @@
       <c r="A59" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="3" t="s">
+      <c r="B60" s="0" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1902,10 +2120,10 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="0" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1942,18 +2160,18 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="4" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1966,18 +2184,18 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="0" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="4" t="s">
         <v>143</v>
       </c>
     </row>
@@ -2014,22 +2232,22 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="0" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B78" s="0" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="16.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
         <v>156</v>
       </c>
@@ -2054,10 +2272,10 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="0" t="s">
         <v>163</v>
       </c>
     </row>
@@ -2078,66 +2296,66 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="4" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
+      <c r="A86" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="0" t="s">
+      <c r="B86" s="4" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
+      <c r="A87" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="B87" s="0" t="s">
+      <c r="B87" s="4" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="0" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="0" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
+      <c r="A90" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B90" s="0" t="s">
+      <c r="B90" s="3" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="0" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
+      <c r="A92" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B92" s="0" t="s">
+      <c r="B92" s="4" t="s">
         <v>183</v>
       </c>
     </row>
@@ -2182,51 +2400,51 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
+      <c r="A98" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="0" t="s">
+      <c r="B98" s="4" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
+      <c r="A99" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="B99" s="0" t="s">
+      <c r="B99" s="3" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B100" s="3" t="s">
+      <c r="A100" s="4" t="s">
         <v>198</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
-        <v>201</v>
-      </c>
-      <c r="B102" s="0" t="s">
+      <c r="A102" s="4" t="s">
         <v>202</v>
       </c>
+      <c r="B102" s="4" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="B103" s="0" t="s">
+      <c r="A103" s="3" t="s">
         <v>204</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2302,18 +2520,18 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="0" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="3" t="s">
+      <c r="A114" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="B114" s="0" t="s">
         <v>226</v>
       </c>
     </row>
@@ -2342,10 +2560,10 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="3" t="s">
+      <c r="A118" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="0" t="s">
         <v>234</v>
       </c>
     </row>
@@ -2358,10 +2576,10 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="0" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2382,583 +2600,822 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="A123" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B123" s="0" t="s">
+      <c r="B123" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="A124" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B124" s="0" t="s">
+      <c r="B124" s="3" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="B125" s="3" t="s">
+      <c r="A125" s="4" t="s">
         <v>247</v>
       </c>
+      <c r="B125" s="4" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
-        <v>248</v>
-      </c>
-      <c r="B126" s="0" t="s">
+      <c r="A126" s="3" t="s">
         <v>249</v>
       </c>
+      <c r="B126" s="3" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="B127" s="3" t="s">
+      <c r="A127" s="0" t="s">
         <v>251</v>
       </c>
+      <c r="B127" s="0" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="B128" s="0" t="s">
+      <c r="A128" s="4" t="s">
         <v>253</v>
       </c>
+      <c r="B128" s="4" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="B129" s="0" t="s">
+      <c r="A129" s="4" t="s">
         <v>255</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="B131" s="0" t="s">
+      <c r="A131" s="3" t="s">
         <v>259</v>
       </c>
+      <c r="B131" s="3" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="B132" s="0" t="s">
+      <c r="A132" s="3" t="s">
         <v>261</v>
       </c>
+      <c r="B132" s="3" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="B133" s="3" t="s">
+      <c r="A133" s="0" t="s">
         <v>263</v>
       </c>
+      <c r="B133" s="0" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="B134" s="0" t="s">
+      <c r="A134" s="3" t="s">
         <v>265</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B135" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B136" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="B137" s="0" t="s">
+      <c r="A137" s="4" t="s">
         <v>271</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B138" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="B139" s="0" t="s">
+      <c r="A139" s="4" t="s">
         <v>275</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B140" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B141" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B142" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B143" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B144" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
-        <v>286</v>
-      </c>
-      <c r="B145" s="0" t="s">
+      <c r="A145" s="4" t="s">
         <v>287</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B146" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B147" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
-        <v>292</v>
-      </c>
-      <c r="B148" s="0" t="s">
+      <c r="A148" s="3" t="s">
         <v>293</v>
       </c>
+      <c r="B148" s="3" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="B149" s="0" t="s">
+      <c r="A149" s="4" t="s">
         <v>295</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B150" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B151" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
-        <v>300</v>
-      </c>
-      <c r="B152" s="0" t="s">
+      <c r="A152" s="4" t="s">
         <v>301</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B153" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B154" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B155" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B156" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B157" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B158" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B159" s="0" t="s">
-        <v>157</v>
+        <v>316</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B160" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B161" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>324</v>
+      <c r="A164" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="B164" s="0" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="B165" s="0" t="s">
-        <v>326</v>
+      <c r="A165" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A167" s="3" t="s">
-        <v>329</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>330</v>
+      <c r="A167" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="B167" s="0" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B175" s="0" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="16.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B176" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B177" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B178" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>354</v>
+      <c r="A179" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="B179" s="0" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="B180" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="3" t="s">
-        <v>357</v>
-      </c>
-      <c r="B181" s="3" t="s">
+      <c r="A181" s="0" t="s">
         <v>358</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B182" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B183" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="B184" s="5" t="s">
+      <c r="A184" s="4" t="s">
         <v>364</v>
       </c>
+      <c r="B184" s="4" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="B185" s="3" t="s">
+      <c r="A185" s="0" t="s">
         <v>366</v>
       </c>
+      <c r="B185" s="0" t="s">
+        <v>367</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="B186" s="3" t="s">
+      <c r="A186" s="0" t="s">
         <v>368</v>
       </c>
+      <c r="B186" s="0" t="s">
+        <v>369</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
-        <v>369</v>
-      </c>
-      <c r="B187" s="0" t="s">
+      <c r="A187" s="4" t="s">
         <v>370</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B188" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B189" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
-        <v>375</v>
-      </c>
-      <c r="B190" s="6" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B190" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>378</v>
+      </c>
+      <c r="B191" s="0" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>380</v>
+      </c>
+      <c r="B192" s="0" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A193" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A194" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>386</v>
+      </c>
+      <c r="B195" s="0" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A196" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>390</v>
+      </c>
+      <c r="B197" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A198" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="B199" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>396</v>
+      </c>
+      <c r="B200" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>398</v>
+      </c>
+      <c r="B201" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>400</v>
+      </c>
+      <c r="B202" s="0" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A203" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="B204" s="0" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A205" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>408</v>
+      </c>
+      <c r="B206" s="0" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A207" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A208" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C208" s="3"/>
+    </row>
+    <row r="209" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A209" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>416</v>
+      </c>
+      <c r="B210" s="0" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>418</v>
+      </c>
+      <c r="B211" s="0" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A212" s="6" t="s">
+        <v>420</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="213" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A213" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A214" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A215" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A216" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A217" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="B218" s="0" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A219" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="B219" s="0" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A220" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A221" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="B221" s="0" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A222" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="B222" s="7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A223" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A224" s="0" t="s">
+        <v>444</v>
+      </c>
+      <c r="B224" s="0" t="s">
+        <v>445</v>
+      </c>
+    </row>
     <row r="225" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="226" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="227" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3718,24 +4175,8 @@
     <row r="981" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="984" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="985" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="986" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="988" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <autoFilter ref="A1:B223"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -3743,5 +4184,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OOP: create Conjecture's class
</commit_message>
<xml_diff>
--- a/data/EngRus.xlsx
+++ b/data/EngRus.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$223</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$224</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$223</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -751,7 +752,7 @@
     <t xml:space="preserve">issue</t>
   </si>
   <si>
-    <t xml:space="preserve">вопрос, исход, результат, выдавать выпускать</t>
+    <t xml:space="preserve">вопрос, исход, результат, выдавать, выпускать</t>
   </si>
   <si>
     <t xml:space="preserve">it happens</t>
@@ -1610,9 +1611,9 @@
   <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B218" activeCellId="0" sqref="B218"/>
+      <selection pane="bottomLeft" activeCell="B118" activeCellId="0" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4176,7 +4177,7 @@
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:B223"/>
+  <autoFilter ref="A1:B224"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
a lot of things: redo conjecture's class, add methods of parsing, rework main.rb, rewrite readme
</commit_message>
<xml_diff>
--- a/data/EngRus.xlsx
+++ b/data/EngRus.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$224</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$223</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$223</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$B$224</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -908,7 +908,7 @@
     <t xml:space="preserve">Passed</t>
   </si>
   <si>
-    <t xml:space="preserve">Миновал</t>
+    <t xml:space="preserve">Миновал, прошёл</t>
   </si>
   <si>
     <t xml:space="preserve">permission</t>
@@ -1611,9 +1611,9 @@
   <dimension ref="A1:C225"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B118" activeCellId="0" sqref="B118"/>
+      <selection pane="bottomLeft" activeCell="B149" activeCellId="0" sqref="B149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4177,7 +4177,7 @@
     <row r="982" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="983" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:B224"/>
+  <autoFilter ref="A1:B223"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>